<commit_message>
finishing up version 1.0
</commit_message>
<xml_diff>
--- a/CheckEntry/Checks.xlsx
+++ b/CheckEntry/Checks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KTM\python\msutils\CheckEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37B55A-8219-483E-BC1A-6001DEBBD533}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1201D1-46B2-406C-9FA5-2739958601E9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9465" xr2:uid="{AEAB3ED2-E40E-4194-BDC3-A483C024D04A}"/>
   </bookViews>
@@ -30,21 +30,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>Snyder, Richard</t>
-  </si>
-  <si>
-    <t>Alpert, Alan</t>
-  </si>
-  <si>
-    <t>Fox, Robert</t>
-  </si>
-  <si>
-    <t>Schlossberg,Sam</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Segal, Paul</t>
+  </si>
+  <si>
+    <t>Levenson, David</t>
+  </si>
+  <si>
+    <t>Matzkin, Harold</t>
+  </si>
+  <si>
+    <t>Shnayder, Leon</t>
+  </si>
+  <si>
+    <t>Sokolinski, Ilia</t>
+  </si>
+  <si>
+    <t>Berkovits, Shimshon</t>
+  </si>
+  <si>
+    <t>Gordon, Victorine</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4BE3D9-2412-4FA3-B7DC-389623A5E759}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,27 +420,32 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>